<commit_message>
bat dau làm chuc nang khoa hoc
</commit_message>
<xml_diff>
--- a/database/seeders/_seeder.xlsx
+++ b/database/seeders/_seeder.xlsx
@@ -5,15 +5,20 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\source\repos\TeKy_DoAn\database\seeders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\source\repos\DoAn_Final\database\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Users" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoc_Sinh" sheetId="2" r:id="rId2"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="phu_huynh" sheetId="8" r:id="rId2"/>
+    <sheet name="hoc_sinh" sheetId="2" r:id="rId3"/>
+    <sheet name="giao_vien" sheetId="7" r:id="rId4"/>
+    <sheet name="level" sheetId="4" r:id="rId5"/>
+    <sheet name="loai_khoa_hoc" sheetId="5" r:id="rId6"/>
+    <sheet name="khoa_hoc" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -42,9 +47,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>default.png</t>
-  </si>
-  <si>
     <t>cuong1998pro</t>
   </si>
   <si>
@@ -72,17 +74,240 @@
     <t>hodem</t>
   </si>
   <si>
-    <t>pham</t>
+    <t>$2y$10$l4cAzWxFQei93wJEUm4KMuZGrxwxuPpO285RiLdf6Gm8Aaf7cwj5W</t>
+  </si>
+  <si>
+    <t>$2y$10$cMX0hcjDo8g3R0F.shZd3.5F9Y3F4e2n4feD2eMuth3NG7FhyWDrW</t>
+  </si>
+  <si>
+    <t>$2y$10$LkmpS6uCMm6Lg3V2q/6oRu4S1oXofMotTFLENgDg6qzYSd/cY9slq</t>
+  </si>
+  <si>
+    <t>$2y$10$KMjVDbnMwv28Rf6fFnfDluM7z01hX0tRxVgUMGh5fT6fVAzPqpram</t>
+  </si>
+  <si>
+    <t>asset/jpg/avatar-1.jpg</t>
+  </si>
+  <si>
+    <t>asset/jpg/avatar-2.jpg</t>
+  </si>
+  <si>
+    <t>asset/jpg/avatar-5.jpg</t>
+  </si>
+  <si>
+    <t>asset/jpg/avatar-4.jpg</t>
+  </si>
+  <si>
+    <t>cmnd</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sodienthoai</t>
+  </si>
+  <si>
+    <t>ngaysinh</t>
+  </si>
+  <si>
+    <t>gioitinh</t>
+  </si>
+  <si>
+    <t>diachi</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>asset/jpg/avatar-3.jpg</t>
+  </si>
+  <si>
+    <t>phuhuynh01</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy6</t>
+  </si>
+  <si>
+    <t>hocsinh01</t>
+  </si>
+  <si>
+    <t>hocsinh02</t>
+  </si>
+  <si>
+    <t>23/5B đường Lê Lợi, Phường 6, thành phố Tuy Hòa, tỉnh Phú Yên</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Khánh</t>
+  </si>
+  <si>
+    <t>Phạm Văn</t>
+  </si>
+  <si>
+    <t>tenkhoahoc</t>
+  </si>
+  <si>
+    <t>dotuoi</t>
+  </si>
+  <si>
+    <t>sisotoida</t>
+  </si>
+  <si>
+    <t>dieukienhoc</t>
+  </si>
+  <si>
+    <t>hocphi</t>
+  </si>
+  <si>
+    <t>loai_khoa_hoc_id</t>
+  </si>
+  <si>
+    <t>level_id</t>
+  </si>
+  <si>
+    <t>tenlevel</t>
+  </si>
+  <si>
+    <t>mota</t>
+  </si>
+  <si>
+    <t>Sơ cấp</t>
+  </si>
+  <si>
+    <t>Trung cấp</t>
+  </si>
+  <si>
+    <t>Khóa học dành cho các bé mới bắt đầu tiếp cận</t>
+  </si>
+  <si>
+    <t>Cao cấp</t>
+  </si>
+  <si>
+    <t>Khóa học dành cho các bé đã hoàn thành mức độ trung cấp</t>
+  </si>
+  <si>
+    <t>Khóa học dành cho các bé đã hoàn thành mức độ sơ cấp</t>
+  </si>
+  <si>
+    <t>tenloaikhoahoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lập trình &amp; Phát triển ứng dụng </t>
+  </si>
+  <si>
+    <t>Scratch Jr là ngôn ngữ lập trình kéo thả trực quan dành cho độ tuổi 4-5 để làm quen với tư duy lập trình, chủ yếu giúp phát triển sự sáng tạo, tư duy logic của trẻ em qua việc tạo ra các sản phẩm, câu chuyện và trò chơi của chính mình.</t>
+  </si>
+  <si>
+    <t>Robot &amp; Điện tử tự động</t>
+  </si>
+  <si>
+    <t>Khoá học này đưa học sinh tiến sâu hơn vào chủ đề Robotics, logics lập trình và thiết kế kiến trúc với Lego Education Wedo. Các em sẽ từng bước dùng các mảnh ghép Lego thực hành với ròng rọc, động cơ, các loại cảm ứng để tạo nên các robot là các nhân vật.</t>
+  </si>
+  <si>
+    <t>3D &amp; Truyền thông đa phương tiện</t>
+  </si>
+  <si>
+    <t>Khoá học dựng hình, vẽ và in 3D được thiết kế từ trình độ sơ cấp tới nâng cao cho học sinh độ tuổi 7-10. Đây là lựa chọn hoàn hảo cho những học sinh thích hoạt động sáng tạo và muốn tạo ra từ các mô hình thực tế, thông qua sử dụng phần mềm.</t>
+  </si>
+  <si>
+    <t>Khoá học Online</t>
+  </si>
+  <si>
+    <t>Học Online với giáo viên giàu kinh nghiệm, trên nền tảng công nghệ ưu việt, tương tác đa chiều, trải nghiệm thú vị, thuận tiện học tập.</t>
+  </si>
+  <si>
+    <t>MẦM NON CÔNG NGHỆ – LẬP TRÌNH VỚI SCRATCHJR</t>
+  </si>
+  <si>
+    <t>5-7 tuổi</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>noidung</t>
+  </si>
+  <si>
+    <t>Ươm mầm phát triển tư duy logic và sáng tạo trong thời đại số từ 4 tuổi với ngôn ngữ Lập trình Scratch Jr, Robot Uaro, Công nghệ 3D Maker Empire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trong khóa học này, các bạn nhỏ được tiếp cận làm quen với những công nghệ mới nhất của thời đại 4.0, đã có thể tự thiết kế một trò chơi trên máy tính hay chế tạo, điều khiển một chú robot thông qua những công cụ vô cùng hấp dẫn:
+    Ngôn ngữ Scratch Jr là ngôn ngữ lập trình kéo thả trực quan, với thiết kế sinh động, dễ dàng sử dụng và ghi nhớ. Thông qua việc thiết kế và lập trình các nhân vật phim hoạt hình vui nhộn, tạo ra các trò chơi hấp dẫn các bạn nhỏ sẽ bước đầu tiếp cận với khái niệm lập trình, rèn luyện tư duy logic, kỹ năng thiết kế và tư duy giải quyết vấn đề.
+    </t>
+  </si>
+  <si>
+    <t>BÉ LÀM GAME – CẤP 1</t>
+  </si>
+  <si>
+    <t>7 - 10 tuổi</t>
+  </si>
+  <si>
+    <t>Xây dựng đam mê, tạo nền tảng kiến thức Công nghệ; Sử dụng giáo trình xuất sắc tại Mỹ với 50 triệu học sinh &amp; 60,000 trường học trên toàn cầu</t>
+  </si>
+  <si>
+    <t>Be làm Game giúp học sinh tiếp cận, làm quen và phát triển tư duy - khả năng lập trình thông qua chuỗi các môn học - các công cụ coding vô cùng thú vị:
+Lập trình Game 2D với Scratch: Đây là ngôn ngữ lập trình trẻ em phổ biến nhất thế giới, phát triển bởi học viện MIT, Mỹ. Trẻ em tại nhiều quốc gia bắt đầu học lập trình từ 5 tuổi. Công cụ giúp học sinh sáng tạo và phát triển ý tưởng, tăng cường tư duy logic và tiếp cận công nghệ - lập trình một cách tốt nhất. Ngoài ra, học sinh còn được thực hành lập trình trên Robot Truetrue, sản phẩm của Tập đoàn Giáo dục số 1 Hàn Quốc - Sigong Media, phân phối độc quyền bởi Teky.</t>
+  </si>
+  <si>
+    <t>SIÊU NHÂN LẬP TRÌNH WEB – CẤP 2 &amp; CẤP 3</t>
+  </si>
+  <si>
+    <t>12-18 tuổi</t>
+  </si>
+  <si>
+    <t>Phát triển tư duy ứng dụng, sáng tạo cá tính và nuôi dưỡng tinh thần doanh nhân công nghệ trong thời đại 4.0; Theo chuẩn Kiến thức Khoa học máy tính CSTA cho K12 của Mỹ</t>
+  </si>
+  <si>
+    <t>Học sinh sẽ tiếp cận với hoạt động phát triển sản phẩm và ứng dụng công nghệ vào thực tế; ngoài ra học sinh còn được mở rộng các kiến thức liên quan tới khoa học máy tính, bảo mật và hack vốn đang ngày càng trở nên quan trọng hơn trong thế giới công nghệ.
+Python là ngôn ngữ lập trình hướng đối tượng, cấp cao, mạnh mẽ, được sử dụng bởi các công ty công nghệ khổng lồ như Google, Dropbox, Instagram, Quora... nhưng lại vô cùng dễ học. Với cú pháp rất đơn giản, rõ ràng; nó dễ đọc và viết hơn rất nhiều khi so sánh với những ngôn ngữ lập trình khác như C++, Java, C#. Python làm cho việc lập trình trở nên thú vị, cho phép bạn tập trung vào những giải pháp chứ không phải cú pháp. Python đang là xu hướng ngôn ngữ lập trình hàng đầu cho những người mới là</t>
+  </si>
+  <si>
+    <t>Không cần kiến thức lập trình</t>
+  </si>
+  <si>
+    <t>SIÊU NHÂN LẬP TRÌNH APP – CẤP 2 &amp; CẤP 3</t>
+  </si>
+  <si>
+    <t>Học sinh sẽ tiếp cận với hoạt động phát triển sản phẩm và ứng dụng công nghệ vào thực tế; ngoài ra học sinh còn được mở rộng các kiến thức liên quan tới khoa học máy tính, bảo mật và hack vốn đang ngày càng trở nên quan trọng hơn trong thế giới công nghệ.
+App Inventor là một môi trường phát triển tích hợp (IDE) ban đầu được cung cấp bởi Google và hiện được duy trì bởi Viện Công nghệ Massachusetts. Để tạo ra một Ứng dụng di động (Mobile App), bạn không chỉ cần ý tưởng, mà còn cần kiến thức lập trình căn bản cũng như kiến thức sử dụng môi trường phát triển tích hợp để viết lệnh (write code), biên dịch (compile), đóng gói (package), chạy thử (test) hoặc tạo ứng dụng thật (build). Có nhiều môi trường phát triển tích hợp (Integrated Development Envi</t>
+  </si>
+  <si>
+    <t>SIÊU NHÂN LẬP TRÌNH GAME 3D &amp; VR VỚI UNITY – CẤP 2 &amp; CẤP 3</t>
+  </si>
+  <si>
+    <t>11 - 15 tuổi</t>
+  </si>
+  <si>
+    <t>Giáo trình khoá học chuẩn Mỹ, giảng viên tận tình, nội dung học tập chuyên sâu dài hạn</t>
+  </si>
+  <si>
+    <t>Khóa học lập trình Game 3D với Unity giúp học sinh khai phá các ý tưởng kịch bản, trò chơi, xây dựng đồ họa, nhân vật, môi trường trong thế giới 2D, 3D và từ đó phân tích, thiết kế, xây dựng và phát triển các game trên đa nền tảng. Ngoài ra học sinh sẽ tìm hiểu các kiến thức lập trình C# căn bản cũng như kiến thức sử dụng môi trường tích hợp để viết lệnh (write code), biên dịch (compile), đóng gói (package), chạy thử (test) hoặc tạo ứng dụng thật (build).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,13 +330,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,104 +628,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>31444322</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2">
+        <v>337507167</v>
+      </c>
+      <c r="F2" s="2">
+        <v>35806</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>123456</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>123456</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>123456</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>123456</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -495,27 +949,268 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="37.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="55" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1">
+        <v>80000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="1">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="210" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hien thi lop giao vien vao day
</commit_message>
<xml_diff>
--- a/database/seeders/_seeder.xlsx
+++ b/database/seeders/_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="level" sheetId="4" r:id="rId4"/>
     <sheet name="loai_khoa_hoc" sheetId="5" r:id="rId5"/>
     <sheet name="khoa_hoc" sheetId="3" r:id="rId6"/>
-    <sheet name="lop_hoc" sheetId="8" r:id="rId7"/>
+    <sheet name="ca_hoc" sheetId="9" r:id="rId7"/>
+    <sheet name="lop_hoc" sheetId="8" r:id="rId8"/>
+    <sheet name="thoi_khoa_bieu" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="277">
   <si>
     <t>anhdaidien</t>
   </si>
@@ -66,9 +68,6 @@
   </si>
   <si>
     <t>phuhuynh</t>
-  </si>
-  <si>
-    <t>hoatdong</t>
   </si>
   <si>
     <t>hodem</t>
@@ -274,9 +273,6 @@
     <t>Khóa học lập trình Game 3D với Unity giúp học sinh khai phá các ý tưởng kịch bản, trò chơi, xây dựng đồ họa, nhân vật, môi trường trong thế giới 2D, 3D và từ đó phân tích, thiết kế, xây dựng và phát triển các game trên đa nền tảng. Ngoài ra học sinh sẽ tìm hiểu các kiến thức lập trình C# căn bản cũng như kiến thức sử dụng môi trường tích hợp để viết lệnh (write code), biên dịch (compile), đóng gói (package), chạy thử (test) hoặc tạo ứng dụng thật (build).</t>
   </si>
   <si>
-    <t>chinhthuc</t>
-  </si>
-  <si>
     <t>hotenchame</t>
   </si>
   <si>
@@ -493,9 +489,6 @@
     <t>0902489120</t>
   </si>
   <si>
-    <t>hocthu</t>
-  </si>
-  <si>
     <t xml:space="preserve">Đặng Kim </t>
   </si>
   <si>
@@ -713,9 +706,6 @@
   </si>
   <si>
     <t>tenlop</t>
-  </si>
-  <si>
-    <t>danghoatdong</t>
   </si>
   <si>
     <t>ghichu</t>
@@ -769,17 +759,136 @@
     <t>HP-TGVV-0001</t>
   </si>
   <si>
-    <t>daketthuc</t>
+    <t>ngaybatdau</t>
+  </si>
+  <si>
+    <t>ngayketthuc</t>
+  </si>
+  <si>
+    <t>2020/01/09</t>
+  </si>
+  <si>
+    <t>2020/04/10</t>
+  </si>
+  <si>
+    <t>2020/03/20</t>
+  </si>
+  <si>
+    <t>2020/05/12</t>
+  </si>
+  <si>
+    <t>Đã kết thúc</t>
+  </si>
+  <si>
+    <t>Đang hoạt động</t>
+  </si>
+  <si>
+    <t>Chính thức</t>
+  </si>
+  <si>
+    <t>tinhtrang</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>giaovien01</t>
+  </si>
+  <si>
+    <t>giaovien02</t>
+  </si>
+  <si>
+    <t>giaovien03</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy7</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy8</t>
+  </si>
+  <si>
+    <t>$2y$10$wKRif0mHhnAOGZt4Ux1Iq.yyfVFJla5CvmqEXl02XM4FMYj9CYPy9</t>
+  </si>
+  <si>
+    <t>Hoạt động</t>
+  </si>
+  <si>
+    <t>Nguyễn Quỳnh</t>
+  </si>
+  <si>
+    <t>Bùi Lê Hoài</t>
+  </si>
+  <si>
+    <t>Phạm Hồng Bảo</t>
+  </si>
+  <si>
+    <t>Châu</t>
+  </si>
+  <si>
+    <t>1998/01/02</t>
+  </si>
+  <si>
+    <t>1998/01/03</t>
+  </si>
+  <si>
+    <t>1998/01/04</t>
+  </si>
+  <si>
+    <t>031985909</t>
+  </si>
+  <si>
+    <t>031985910</t>
+  </si>
+  <si>
+    <t>031985911</t>
+  </si>
+  <si>
+    <t>0323232332</t>
+  </si>
+  <si>
+    <t>0323232333</t>
+  </si>
+  <si>
+    <t>0323232334</t>
+  </si>
+  <si>
+    <t>cuong1998pro@gmail.com</t>
+  </si>
+  <si>
+    <t>Cơ hữu</t>
+  </si>
+  <si>
+    <t>Cộng tác</t>
+  </si>
+  <si>
+    <t>giao_vien_id</t>
+  </si>
+  <si>
+    <t>thoigianbatdau</t>
+  </si>
+  <si>
+    <t>thoigianketthuc</t>
+  </si>
+  <si>
+    <t>lop_hoc_id</t>
+  </si>
+  <si>
+    <t>ca_hoc_id</t>
+  </si>
+  <si>
+    <t>thu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,6 +976,17 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -876,12 +996,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -905,7 +1040,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -961,15 +1096,34 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="9" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="17" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Bình thường 2" xfId="6"/>
@@ -1267,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1302,121 +1456,172 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1635,7 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1450,802 +1655,802 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75">
       <c r="A2" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I2" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
       <c r="A3" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I3" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.5">
       <c r="A4" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>152</v>
+        <v>245</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I4" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75">
       <c r="A5" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I5" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75">
       <c r="A6" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I6" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75">
       <c r="A7" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I7" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I8" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I9" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I10" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75">
       <c r="A11" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I11" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75">
       <c r="A12" s="9" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I12" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="31.5">
       <c r="A13" s="9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I13" s="16" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75">
       <c r="A14" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I14" s="16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75">
       <c r="A15" s="9" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I15" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
       <c r="A16" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I16" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75">
       <c r="A17" s="9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I17" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75">
       <c r="A18" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I18" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75">
       <c r="A19" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I19" s="16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="31.5">
       <c r="A20" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I20" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="31.5">
       <c r="A21" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I21" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75">
       <c r="A22" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I22" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75">
       <c r="A23" s="9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I23" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75">
       <c r="A24" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I24" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="I25" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75">
@@ -2751,13 +2956,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="17" style="26" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="23"/>
+    <col min="6" max="6" width="14.28515625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="23" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75">
+      <c r="A2" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="J2" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75">
+      <c r="A3" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="J3" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75">
+      <c r="A4" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="J4" s="23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="27"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="27"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="27"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="27"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="27"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="27"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3:G4" r:id="rId2" display="cuong1998pro@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -2766,7 +3137,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2776,34 +3147,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2816,7 +3187,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2826,42 +3197,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
         <v>54</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2873,7 +3244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -2893,51 +3264,51 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="165">
       <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="1">
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1">
         <v>80000</v>
@@ -2951,22 +3322,22 @@
     </row>
     <row r="3" spans="1:9" ht="180">
       <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C3" s="1">
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1">
         <v>1000000</v>
@@ -2980,22 +3351,22 @@
     </row>
     <row r="4" spans="1:9" ht="210">
       <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C4" s="1">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G4" s="1">
         <v>1500000</v>
@@ -3009,22 +3380,22 @@
     </row>
     <row r="5" spans="1:9" ht="210">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1">
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1">
         <v>1500000</v>
@@ -3038,22 +3409,22 @@
     </row>
     <row r="6" spans="1:9" ht="120">
       <c r="A6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C6" s="1">
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="1">
         <v>1500000</v>
@@ -3067,22 +3438,22 @@
     </row>
     <row r="7" spans="1:9" ht="180">
       <c r="A7" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C7" s="1">
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" s="1">
         <v>1500000</v>
@@ -3096,22 +3467,22 @@
     </row>
     <row r="8" spans="1:9" ht="409.5">
       <c r="A8" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1">
         <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="1">
         <v>2000000</v>
@@ -3125,22 +3496,22 @@
     </row>
     <row r="9" spans="1:9" ht="210">
       <c r="A9" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C9" s="1">
         <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="1">
         <v>2000000</v>
@@ -3160,52 +3531,210 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>272</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="30">
+        <v>0.3125</v>
+      </c>
+      <c r="B2" s="31">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="31">
+        <v>0.375</v>
+      </c>
+      <c r="B3" s="31">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="30">
+        <v>0.5625</v>
+      </c>
+      <c r="B4" s="30">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="32">
+        <v>0.625</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0.6875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="32">
+        <v>0.6875</v>
+      </c>
+      <c r="B6" s="32">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="32">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="B7" s="32">
+        <v>0.89583333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
+        <v>271</v>
       </c>
       <c r="C1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="G1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>239</v>
       </c>
+      <c r="E2" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="F2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>240</v>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>241</v>
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>